<commit_message>
add date time parsing
</commit_message>
<xml_diff>
--- a/inst/extdata/xlsx_example.xlsx
+++ b/inst/extdata/xlsx_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -24,16 +24,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
-    <t xml:space="preserve">id</t>
+    <t xml:space="preserve">bio_id</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">data_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_source</t>
+    <t xml:space="preserve">usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source</t>
   </si>
   <si>
     <t xml:space="preserve">location</t>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">44.56694438714396, -123.25117520462796</t>
   </si>
   <si>
-    <t xml:space="preserve">input_type</t>
+    <t xml:space="preserve">type</t>
   </si>
   <si>
     <t xml:space="preserve">reference</t>
@@ -158,12 +158,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,7 +182,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -219,7 +215,7 @@
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -233,7 +229,7 @@
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -244,7 +240,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -256,11 +252,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -273,7 +269,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -286,12 +282,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -302,17 +298,17 @@
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -324,7 +320,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -350,11 +346,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>